<commit_message>
Allinea anagrafiche UO alla versione v2 del controller
- Aggiunta UO KCP (Karol Casa Protetta, Via Sciuti PA)
- KMC, BRG, ROM: stato "In attesa finanziamento" (River Rock), attiva=No
- BET, ZAR: stato "Cliente servizi" (distingue controllate/clienti)
- BRG: posti letto corretti da 0 a 80
- Aggiunto campo StatoUO (Operativa/In attesa/Cliente) e liste filtrate
- Fix Cash_Flow_Strategico: rimosso "=" da etichette testo (causava #NOME!)
- Scadenzario: ridotto a solo header (senza 100 righe vuote)
- Rigenerato Excel Master con 10 UO e correzioni

https://claude.ai/code/session_01JQRNNAKqETTVcrPnRevPxn
</commit_message>
<xml_diff>
--- a/dati/KAROL_CDG_MASTER.xlsx
+++ b/dati/KAROL_CDG_MASTER.xlsx
@@ -38,9 +38,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#.##0,00 €"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -170,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -181,8 +180,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -565,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,8 +576,9 @@
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="55" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -616,10 +614,15 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Stato</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Attiva</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -656,10 +659,15 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
+          <t>Operativa</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
           <t>Sì</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>RSA Alzheimer 44 PL</t>
         </is>
@@ -696,10 +704,15 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
+          <t>Operativa</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
           <t>Sì</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>Psichiatria - Servizi Intensivi/Estensivi + Permessi Terapeutici</t>
         </is>
@@ -736,10 +749,15 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
+          <t>Operativa</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
           <t>Sì</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>Ortopedia/Riabilitazione 50 PL</t>
         </is>
@@ -776,12 +794,17 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Sì</t>
+          <t>In attesa finanziamento</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Day Surgery + Ambulatori</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>Day Surgery + Ambulatori - In attesa finanziamento River Rock</t>
         </is>
       </c>
     </row>
@@ -807,7 +830,7 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
@@ -816,12 +839,17 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Sì</t>
+          <t>In attesa finanziamento</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>RSA + FKT + Centro Diurno</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>RSA 80 PL + FKT + Centro Diurno - In attesa finanziamento River Rock</t>
         </is>
       </c>
     </row>
@@ -856,12 +884,17 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Sì</t>
+          <t>In attesa finanziamento</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>Riabilitazione 77 PL</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>Riabilitazione 77 PL - In attesa finanziamento River Rock</t>
         </is>
       </c>
     </row>
@@ -896,10 +929,15 @@
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
+          <t>Operativa</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
           <t>Sì</t>
         </is>
       </c>
-      <c r="H8" s="2" t="inlineStr">
+      <c r="I8" s="2" t="inlineStr">
         <is>
           <t>Laboratori Analisi</t>
         </is>
@@ -936,12 +974,17 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
+          <t>Cliente servizi</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
           <t>Sì</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>11 strutture RSA/Riabilitazione</t>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>11 strutture RSA/Riabilitazione - Cliente servizi</t>
         </is>
       </c>
     </row>
@@ -976,12 +1019,62 @@
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
+          <t>Cliente servizi</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
           <t>Sì</t>
         </is>
       </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>Servizi ristorazione</t>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>Servizi ristorazione - Cliente servizi sede</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>KCP</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Karol Casa Protetta</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>RSA Non Autosufficienti</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Sicilia</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>Karol S.p.A.</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>Operativa</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>Sì</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>Via Sciuti PA</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1107,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>CONTO ECONOMICO CONSOLIDATO - GRUPPO KAROL</t>
         </is>
@@ -1097,7 +1190,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>CASH FLOW OPERATIVO - ROLLING 1-3 MESI</t>
         </is>
@@ -1146,7 +1239,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="inlineStr">
+      <c r="A4" s="15" t="inlineStr">
         <is>
           <t>CASSA INIZIALE</t>
         </is>
@@ -1156,7 +1249,7 @@
       <c r="A5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t>INCASSI</t>
         </is>
@@ -1191,24 +1284,24 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="20" t="inlineStr">
+      <c r="A11" s="18" t="inlineStr">
         <is>
           <t>TOTALE INCASSI</t>
         </is>
       </c>
-      <c r="B11" s="19" t="n"/>
-      <c r="C11" s="19" t="n"/>
-      <c r="D11" s="19" t="n"/>
-      <c r="E11" s="19" t="n"/>
-      <c r="F11" s="19" t="n"/>
-      <c r="G11" s="19" t="n"/>
-      <c r="H11" s="19" t="n"/>
+      <c r="B11" s="17" t="n"/>
+      <c r="C11" s="17" t="n"/>
+      <c r="D11" s="17" t="n"/>
+      <c r="E11" s="17" t="n"/>
+      <c r="F11" s="17" t="n"/>
+      <c r="G11" s="17" t="n"/>
+      <c r="H11" s="17" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="inlineStr">
+      <c r="A13" s="15" t="inlineStr">
         <is>
           <t>PAGAMENTI</t>
         </is>
@@ -1257,42 +1350,42 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="20" t="inlineStr">
+      <c r="A20" s="18" t="inlineStr">
         <is>
           <t>TOTALE PAGAMENTI</t>
         </is>
       </c>
-      <c r="B20" s="19" t="n"/>
-      <c r="C20" s="19" t="n"/>
-      <c r="D20" s="19" t="n"/>
-      <c r="E20" s="19" t="n"/>
-      <c r="F20" s="19" t="n"/>
-      <c r="G20" s="19" t="n"/>
-      <c r="H20" s="19" t="n"/>
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="17" t="n"/>
+      <c r="D20" s="17" t="n"/>
+      <c r="E20" s="17" t="n"/>
+      <c r="F20" s="17" t="n"/>
+      <c r="G20" s="17" t="n"/>
+      <c r="H20" s="17" t="n"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="17" t="inlineStr">
+      <c r="A22" s="15" t="inlineStr">
         <is>
           <t>SALDO PERIODO</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="20" t="inlineStr">
+      <c r="A23" s="18" t="inlineStr">
         <is>
           <t>CASSA FINALE</t>
         </is>
       </c>
-      <c r="B23" s="19" t="n"/>
-      <c r="C23" s="19" t="n"/>
-      <c r="D23" s="19" t="n"/>
-      <c r="E23" s="19" t="n"/>
-      <c r="F23" s="19" t="n"/>
-      <c r="G23" s="19" t="n"/>
-      <c r="H23" s="19" t="n"/>
+      <c r="B23" s="17" t="n"/>
+      <c r="C23" s="17" t="n"/>
+      <c r="D23" s="17" t="n"/>
+      <c r="E23" s="17" t="n"/>
+      <c r="F23" s="17" t="n"/>
+      <c r="G23" s="17" t="n"/>
+      <c r="H23" s="17" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1325,7 +1418,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>CASH FLOW STRATEGICO - PIANO 5 ANNI</t>
         </is>
@@ -1385,15 +1478,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="20">
-        <f> FREE CASH FLOW OPERATIVO</f>
-        <v/>
-      </c>
-      <c r="B7" s="19" t="n"/>
-      <c r="C7" s="19" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="19" t="n"/>
-      <c r="F7" s="19" t="n"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FREE CASH FLOW OPERATIVO</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1413,54 +1502,50 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="20">
-        <f> FREE CASH FLOW NETTO</f>
-        <v/>
-      </c>
-      <c r="B11" s="19" t="n"/>
-      <c r="C11" s="19" t="n"/>
-      <c r="D11" s="19" t="n"/>
-      <c r="E11" s="19" t="n"/>
-      <c r="F11" s="19" t="n"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FREE CASH FLOW NETTO</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="20" t="inlineStr">
+      <c r="A13" s="18" t="inlineStr">
         <is>
           <t>PFN iniziale</t>
         </is>
       </c>
-      <c r="B13" s="19" t="n"/>
-      <c r="C13" s="19" t="n"/>
-      <c r="D13" s="19" t="n"/>
-      <c r="E13" s="19" t="n"/>
-      <c r="F13" s="19" t="n"/>
+      <c r="B13" s="17" t="n"/>
+      <c r="C13" s="17" t="n"/>
+      <c r="D13" s="17" t="n"/>
+      <c r="E13" s="17" t="n"/>
+      <c r="F13" s="17" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="20" t="inlineStr">
+      <c r="A14" s="18" t="inlineStr">
         <is>
           <t>PFN finale</t>
         </is>
       </c>
-      <c r="B14" s="19" t="n"/>
-      <c r="C14" s="19" t="n"/>
-      <c r="D14" s="19" t="n"/>
-      <c r="E14" s="19" t="n"/>
-      <c r="F14" s="19" t="n"/>
+      <c r="B14" s="17" t="n"/>
+      <c r="C14" s="17" t="n"/>
+      <c r="D14" s="17" t="n"/>
+      <c r="E14" s="17" t="n"/>
+      <c r="F14" s="17" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="20" t="inlineStr">
+      <c r="A15" s="18" t="inlineStr">
         <is>
           <t>PFN/EBITDA</t>
         </is>
       </c>
-      <c r="B15" s="19" t="n"/>
-      <c r="C15" s="19" t="n"/>
-      <c r="D15" s="19" t="n"/>
-      <c r="E15" s="19" t="n"/>
-      <c r="F15" s="19" t="n"/>
+      <c r="B15" s="17" t="n"/>
+      <c r="C15" s="17" t="n"/>
+      <c r="D15" s="17" t="n"/>
+      <c r="E15" s="17" t="n"/>
+      <c r="F15" s="17" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1495,7 +1580,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>KPI - INDICATORI CHIAVE DI PERFORMANCE</t>
         </is>
@@ -1564,7 +1649,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1584,10 +1669,11 @@
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="12" customWidth="1" min="11" max="11"/>
     <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>REGOLE DI ALLOCAZIONE COSTI SEDE</t>
         </is>
@@ -1652,6 +1738,11 @@
       <c r="L3" s="1" t="inlineStr">
         <is>
           <t>ZAR</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>KCP</t>
         </is>
       </c>
     </row>
@@ -1680,6 +1771,7 @@
       <c r="J4" s="7" t="n"/>
       <c r="K4" s="7" t="n"/>
       <c r="L4" s="7" t="n"/>
+      <c r="M4" s="7" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1706,6 +1798,7 @@
       <c r="J5" s="7" t="n"/>
       <c r="K5" s="7" t="n"/>
       <c r="L5" s="7" t="n"/>
+      <c r="M5" s="7" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1732,6 +1825,7 @@
       <c r="J6" s="7" t="n"/>
       <c r="K6" s="7" t="n"/>
       <c r="L6" s="7" t="n"/>
+      <c r="M6" s="7" t="n"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1758,6 +1852,7 @@
       <c r="J7" s="7" t="n"/>
       <c r="K7" s="7" t="n"/>
       <c r="L7" s="7" t="n"/>
+      <c r="M7" s="7" t="n"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1784,6 +1879,7 @@
       <c r="J8" s="7" t="n"/>
       <c r="K8" s="7" t="n"/>
       <c r="L8" s="7" t="n"/>
+      <c r="M8" s="7" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1810,6 +1906,7 @@
       <c r="J9" s="7" t="n"/>
       <c r="K9" s="7" t="n"/>
       <c r="L9" s="7" t="n"/>
+      <c r="M9" s="7" t="n"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1836,6 +1933,7 @@
       <c r="J10" s="7" t="n"/>
       <c r="K10" s="7" t="n"/>
       <c r="L10" s="7" t="n"/>
+      <c r="M10" s="7" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1862,6 +1960,7 @@
       <c r="J11" s="7" t="n"/>
       <c r="K11" s="7" t="n"/>
       <c r="L11" s="7" t="n"/>
+      <c r="M11" s="7" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1888,6 +1987,7 @@
       <c r="J12" s="7" t="n"/>
       <c r="K12" s="7" t="n"/>
       <c r="L12" s="7" t="n"/>
+      <c r="M12" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1921,7 +2021,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>BENCHMARK DI SETTORE - COSTI STANDARD</t>
         </is>
@@ -2151,7 +2251,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>PARAMETRI SCENARI CASH FLOW</t>
         </is>
@@ -2180,7 +2280,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>DSO ASP (giorni)</t>
         </is>
@@ -2196,7 +2296,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Delta Occupancy</t>
         </is>
@@ -2212,7 +2312,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>Costi imprevisti %</t>
         </is>
@@ -2228,7 +2328,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Crescita ricavi %</t>
         </is>
@@ -2271,7 +2371,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>CONFIGURAZIONE SOGLIE ALERT</t>
         </is>
@@ -2300,7 +2400,7 @@
           <t>cassa_minima</t>
         </is>
       </c>
-      <c r="B4" s="24" t="n">
+      <c r="B4" s="22" t="n">
         <v>200000</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -2315,7 +2415,7 @@
           <t>copertura_minima_giorni</t>
         </is>
       </c>
-      <c r="B5" s="24" t="n">
+      <c r="B5" s="22" t="n">
         <v>30</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
@@ -2330,7 +2430,7 @@
           <t>dso_massimo_asp</t>
         </is>
       </c>
-      <c r="B6" s="24" t="n">
+      <c r="B6" s="22" t="n">
         <v>150</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -2345,7 +2445,7 @@
           <t>dso_massimo_privati</t>
         </is>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="22" t="n">
         <v>60</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
@@ -2360,7 +2460,7 @@
           <t>dpo_massimo_fornitori</t>
         </is>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="22" t="n">
         <v>120</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
@@ -2375,7 +2475,7 @@
           <t>dscr_minimo</t>
         </is>
       </c>
-      <c r="B9" s="24" t="n">
+      <c r="B9" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="inlineStr">
@@ -2390,7 +2490,7 @@
           <t>mol_minimo_uo</t>
         </is>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="22" t="n">
         <v>0.05</v>
       </c>
       <c r="C10" s="2" t="inlineStr">
@@ -2405,7 +2505,7 @@
           <t>mol_minimo_consolidato</t>
         </is>
       </c>
-      <c r="B11" s="24" t="n">
+      <c r="B11" s="22" t="n">
         <v>0.08</v>
       </c>
       <c r="C11" s="2" t="inlineStr">
@@ -2420,7 +2520,7 @@
           <t>costo_personale_max_pct</t>
         </is>
       </c>
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="22" t="n">
         <v>0.6</v>
       </c>
       <c r="C12" s="2" t="inlineStr">
@@ -2435,7 +2535,7 @@
           <t>peso_costi_sede_max_pct</t>
         </is>
       </c>
-      <c r="B13" s="24" t="n">
+      <c r="B13" s="22" t="n">
         <v>0.2</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
@@ -2450,7 +2550,7 @@
           <t>scostamento_budget_max</t>
         </is>
       </c>
-      <c r="B14" s="24" t="n">
+      <c r="B14" s="22" t="n">
         <v>0.1</v>
       </c>
       <c r="C14" s="2" t="inlineStr">
@@ -2465,7 +2565,7 @@
           <t>occupancy_minima</t>
         </is>
       </c>
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="22" t="n">
         <v>0.8</v>
       </c>
       <c r="C15" s="2" t="inlineStr">
@@ -2480,7 +2580,7 @@
           <t>scostamento_ricavo_giornata</t>
         </is>
       </c>
-      <c r="B16" s="24" t="n">
+      <c r="B16" s="22" t="n">
         <v>0.1</v>
       </c>
       <c r="C16" s="2" t="inlineStr">
@@ -2495,7 +2595,7 @@
           <t>scostamento_costo_giornata</t>
         </is>
       </c>
-      <c r="B17" s="24" t="n">
+      <c r="B17" s="22" t="n">
         <v>0.1</v>
       </c>
       <c r="C17" s="2" t="inlineStr">
@@ -2537,51 +2637,51 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>SCENARIO 1</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="15" t="inlineStr">
         <is>
           <t>Nome:</t>
         </is>
       </c>
-      <c r="B3" s="25" t="inlineStr"/>
+      <c r="B3" s="23" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="inlineStr">
+      <c r="A4" s="15" t="inlineStr">
         <is>
           <t>Descrizione:</t>
         </is>
       </c>
-      <c r="B4" s="25" t="inlineStr"/>
+      <c r="B4" s="23" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="inlineStr">
+      <c r="A5" s="15" t="inlineStr">
         <is>
           <t>Stato:</t>
         </is>
       </c>
-      <c r="B5" s="25" t="inlineStr">
+      <c r="B5" s="23" t="inlineStr">
         <is>
           <t>Bozza</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t>Data Creazione:</t>
         </is>
       </c>
-      <c r="B6" s="25" t="inlineStr"/>
+      <c r="B6" s="23" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="inlineStr"/>
-      <c r="B7" s="25" t="inlineStr"/>
+      <c r="A7" s="15" t="inlineStr"/>
+      <c r="B7" s="23" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -2745,7 +2845,7 @@
           <t>Delta Ricavi</t>
         </is>
       </c>
-      <c r="B23" s="25" t="n"/>
+      <c r="B23" s="23" t="n"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2753,7 +2853,7 @@
           <t>Delta Costi</t>
         </is>
       </c>
-      <c r="B24" s="25" t="n"/>
+      <c r="B24" s="23" t="n"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2761,7 +2861,7 @@
           <t>Delta MOL</t>
         </is>
       </c>
-      <c r="B25" s="25" t="n"/>
+      <c r="B25" s="23" t="n"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2769,11 +2869,11 @@
           <t>Delta MOL %</t>
         </is>
       </c>
-      <c r="B26" s="25" t="n"/>
+      <c r="B26" s="23" t="n"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
-      <c r="B27" s="25" t="n"/>
+      <c r="B27" s="23" t="n"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2781,7 +2881,7 @@
           <t>Investimento Richiesto</t>
         </is>
       </c>
-      <c r="B28" s="25" t="n"/>
+      <c r="B28" s="23" t="n"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2789,7 +2889,7 @@
           <t>Payback (mesi)</t>
         </is>
       </c>
-      <c r="B29" s="25" t="n"/>
+      <c r="B29" s="23" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2797,7 +2897,7 @@
           <t>Impatto Cassa Anno 1</t>
         </is>
       </c>
-      <c r="B30" s="25" t="n"/>
+      <c r="B30" s="23" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2832,51 +2932,51 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>SCENARIO 2</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="15" t="inlineStr">
         <is>
           <t>Nome:</t>
         </is>
       </c>
-      <c r="B3" s="25" t="inlineStr"/>
+      <c r="B3" s="23" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="inlineStr">
+      <c r="A4" s="15" t="inlineStr">
         <is>
           <t>Descrizione:</t>
         </is>
       </c>
-      <c r="B4" s="25" t="inlineStr"/>
+      <c r="B4" s="23" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="inlineStr">
+      <c r="A5" s="15" t="inlineStr">
         <is>
           <t>Stato:</t>
         </is>
       </c>
-      <c r="B5" s="25" t="inlineStr">
+      <c r="B5" s="23" t="inlineStr">
         <is>
           <t>Bozza</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t>Data Creazione:</t>
         </is>
       </c>
-      <c r="B6" s="25" t="inlineStr"/>
+      <c r="B6" s="23" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="inlineStr"/>
-      <c r="B7" s="25" t="inlineStr"/>
+      <c r="A7" s="15" t="inlineStr"/>
+      <c r="B7" s="23" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -3040,7 +3140,7 @@
           <t>Delta Ricavi</t>
         </is>
       </c>
-      <c r="B23" s="25" t="n"/>
+      <c r="B23" s="23" t="n"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3048,7 +3148,7 @@
           <t>Delta Costi</t>
         </is>
       </c>
-      <c r="B24" s="25" t="n"/>
+      <c r="B24" s="23" t="n"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3056,7 +3156,7 @@
           <t>Delta MOL</t>
         </is>
       </c>
-      <c r="B25" s="25" t="n"/>
+      <c r="B25" s="23" t="n"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3064,11 +3164,11 @@
           <t>Delta MOL %</t>
         </is>
       </c>
-      <c r="B26" s="25" t="n"/>
+      <c r="B26" s="23" t="n"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
-      <c r="B27" s="25" t="n"/>
+      <c r="B27" s="23" t="n"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3076,7 +3176,7 @@
           <t>Investimento Richiesto</t>
         </is>
       </c>
-      <c r="B28" s="25" t="n"/>
+      <c r="B28" s="23" t="n"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3084,7 +3184,7 @@
           <t>Payback (mesi)</t>
         </is>
       </c>
-      <c r="B29" s="25" t="n"/>
+      <c r="B29" s="23" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3092,7 +3192,7 @@
           <t>Impatto Cassa Anno 1</t>
         </is>
       </c>
-      <c r="B30" s="25" t="n"/>
+      <c r="B30" s="23" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3199,51 +3299,51 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>SCENARIO 3</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="15" t="inlineStr">
         <is>
           <t>Nome:</t>
         </is>
       </c>
-      <c r="B3" s="25" t="inlineStr"/>
+      <c r="B3" s="23" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="inlineStr">
+      <c r="A4" s="15" t="inlineStr">
         <is>
           <t>Descrizione:</t>
         </is>
       </c>
-      <c r="B4" s="25" t="inlineStr"/>
+      <c r="B4" s="23" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="inlineStr">
+      <c r="A5" s="15" t="inlineStr">
         <is>
           <t>Stato:</t>
         </is>
       </c>
-      <c r="B5" s="25" t="inlineStr">
+      <c r="B5" s="23" t="inlineStr">
         <is>
           <t>Bozza</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="inlineStr">
+      <c r="A6" s="15" t="inlineStr">
         <is>
           <t>Data Creazione:</t>
         </is>
       </c>
-      <c r="B6" s="25" t="inlineStr"/>
+      <c r="B6" s="23" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="inlineStr"/>
-      <c r="B7" s="25" t="inlineStr"/>
+      <c r="A7" s="15" t="inlineStr"/>
+      <c r="B7" s="23" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -3407,7 +3507,7 @@
           <t>Delta Ricavi</t>
         </is>
       </c>
-      <c r="B23" s="25" t="n"/>
+      <c r="B23" s="23" t="n"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3415,7 +3515,7 @@
           <t>Delta Costi</t>
         </is>
       </c>
-      <c r="B24" s="25" t="n"/>
+      <c r="B24" s="23" t="n"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3423,7 +3523,7 @@
           <t>Delta MOL</t>
         </is>
       </c>
-      <c r="B25" s="25" t="n"/>
+      <c r="B25" s="23" t="n"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3431,11 +3531,11 @@
           <t>Delta MOL %</t>
         </is>
       </c>
-      <c r="B26" s="25" t="n"/>
+      <c r="B26" s="23" t="n"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
-      <c r="B27" s="25" t="n"/>
+      <c r="B27" s="23" t="n"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3443,7 +3543,7 @@
           <t>Investimento Richiesto</t>
         </is>
       </c>
-      <c r="B28" s="25" t="n"/>
+      <c r="B28" s="23" t="n"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3451,7 +3551,7 @@
           <t>Payback (mesi)</t>
         </is>
       </c>
-      <c r="B29" s="25" t="n"/>
+      <c r="B29" s="23" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3459,7 +3559,7 @@
           <t>Impatto Cassa Anno 1</t>
         </is>
       </c>
-      <c r="B30" s="25" t="n"/>
+      <c r="B30" s="23" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3487,14 +3587,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>DASHBOARD OPERATIVA - KPI PER UNITÀ OPERATIVA</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="26" t="inlineStr">
+      <c r="A3" s="24" t="inlineStr">
         <is>
           <t>Periodo: [Aggiornato automaticamente]</t>
         </is>
@@ -3533,14 +3633,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>DASHBOARD ECONOMICA - CE E MARGINI</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="26" t="inlineStr">
+      <c r="A3" s="24" t="inlineStr">
         <is>
           <t>Periodo: [Aggiornato automaticamente]</t>
         </is>
@@ -3579,14 +3679,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>DASHBOARD FINANZIARIA - CASH FLOW E POSIZIONE</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="26" t="inlineStr">
+      <c r="A3" s="24" t="inlineStr">
         <is>
           <t>Periodo: [Aggiornato automaticamente]</t>
         </is>
@@ -4785,7 +4885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4844,1006 +4944,6 @@
           <t>Note</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="n"/>
-      <c r="B2" s="7" t="n"/>
-      <c r="C2" s="7" t="n"/>
-      <c r="D2" s="9" t="n"/>
-      <c r="E2" s="7" t="n"/>
-      <c r="F2" s="7" t="n"/>
-      <c r="G2" s="7" t="n"/>
-      <c r="H2" s="7" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n"/>
-      <c r="B3" s="7" t="n"/>
-      <c r="C3" s="7" t="n"/>
-      <c r="D3" s="9" t="n"/>
-      <c r="E3" s="7" t="n"/>
-      <c r="F3" s="7" t="n"/>
-      <c r="G3" s="7" t="n"/>
-      <c r="H3" s="7" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n"/>
-      <c r="B4" s="7" t="n"/>
-      <c r="C4" s="7" t="n"/>
-      <c r="D4" s="9" t="n"/>
-      <c r="E4" s="7" t="n"/>
-      <c r="F4" s="7" t="n"/>
-      <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n"/>
-      <c r="B5" s="7" t="n"/>
-      <c r="C5" s="7" t="n"/>
-      <c r="D5" s="9" t="n"/>
-      <c r="E5" s="7" t="n"/>
-      <c r="F5" s="7" t="n"/>
-      <c r="G5" s="7" t="n"/>
-      <c r="H5" s="7" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="n"/>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="7" t="n"/>
-      <c r="D6" s="9" t="n"/>
-      <c r="E6" s="7" t="n"/>
-      <c r="F6" s="7" t="n"/>
-      <c r="G6" s="7" t="n"/>
-      <c r="H6" s="7" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="n"/>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="9" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="7" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="n"/>
-      <c r="B8" s="7" t="n"/>
-      <c r="C8" s="7" t="n"/>
-      <c r="D8" s="9" t="n"/>
-      <c r="E8" s="7" t="n"/>
-      <c r="F8" s="7" t="n"/>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="7" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="n"/>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="7" t="n"/>
-      <c r="D9" s="9" t="n"/>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="7" t="n"/>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="7" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="n"/>
-      <c r="B10" s="7" t="n"/>
-      <c r="C10" s="7" t="n"/>
-      <c r="D10" s="9" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="8" t="n"/>
-      <c r="B11" s="7" t="n"/>
-      <c r="C11" s="7" t="n"/>
-      <c r="D11" s="9" t="n"/>
-      <c r="E11" s="7" t="n"/>
-      <c r="F11" s="7" t="n"/>
-      <c r="G11" s="7" t="n"/>
-      <c r="H11" s="7" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="n"/>
-      <c r="B12" s="7" t="n"/>
-      <c r="C12" s="7" t="n"/>
-      <c r="D12" s="9" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="n"/>
-      <c r="B13" s="7" t="n"/>
-      <c r="C13" s="7" t="n"/>
-      <c r="D13" s="9" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="7" t="n"/>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="8" t="n"/>
-      <c r="B14" s="7" t="n"/>
-      <c r="C14" s="7" t="n"/>
-      <c r="D14" s="9" t="n"/>
-      <c r="E14" s="7" t="n"/>
-      <c r="F14" s="7" t="n"/>
-      <c r="G14" s="7" t="n"/>
-      <c r="H14" s="7" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="n"/>
-      <c r="B15" s="7" t="n"/>
-      <c r="C15" s="7" t="n"/>
-      <c r="D15" s="9" t="n"/>
-      <c r="E15" s="7" t="n"/>
-      <c r="F15" s="7" t="n"/>
-      <c r="G15" s="7" t="n"/>
-      <c r="H15" s="7" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="8" t="n"/>
-      <c r="B16" s="7" t="n"/>
-      <c r="C16" s="7" t="n"/>
-      <c r="D16" s="9" t="n"/>
-      <c r="E16" s="7" t="n"/>
-      <c r="F16" s="7" t="n"/>
-      <c r="G16" s="7" t="n"/>
-      <c r="H16" s="7" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="8" t="n"/>
-      <c r="B17" s="7" t="n"/>
-      <c r="C17" s="7" t="n"/>
-      <c r="D17" s="9" t="n"/>
-      <c r="E17" s="7" t="n"/>
-      <c r="F17" s="7" t="n"/>
-      <c r="G17" s="7" t="n"/>
-      <c r="H17" s="7" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="8" t="n"/>
-      <c r="B18" s="7" t="n"/>
-      <c r="C18" s="7" t="n"/>
-      <c r="D18" s="9" t="n"/>
-      <c r="E18" s="7" t="n"/>
-      <c r="F18" s="7" t="n"/>
-      <c r="G18" s="7" t="n"/>
-      <c r="H18" s="7" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="8" t="n"/>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="D19" s="9" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="8" t="n"/>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-      <c r="D20" s="9" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="7" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="8" t="n"/>
-      <c r="B21" s="7" t="n"/>
-      <c r="C21" s="7" t="n"/>
-      <c r="D21" s="9" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="7" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="8" t="n"/>
-      <c r="B22" s="7" t="n"/>
-      <c r="C22" s="7" t="n"/>
-      <c r="D22" s="9" t="n"/>
-      <c r="E22" s="7" t="n"/>
-      <c r="F22" s="7" t="n"/>
-      <c r="G22" s="7" t="n"/>
-      <c r="H22" s="7" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="8" t="n"/>
-      <c r="B23" s="7" t="n"/>
-      <c r="C23" s="7" t="n"/>
-      <c r="D23" s="9" t="n"/>
-      <c r="E23" s="7" t="n"/>
-      <c r="F23" s="7" t="n"/>
-      <c r="G23" s="7" t="n"/>
-      <c r="H23" s="7" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="8" t="n"/>
-      <c r="B24" s="7" t="n"/>
-      <c r="C24" s="7" t="n"/>
-      <c r="D24" s="9" t="n"/>
-      <c r="E24" s="7" t="n"/>
-      <c r="F24" s="7" t="n"/>
-      <c r="G24" s="7" t="n"/>
-      <c r="H24" s="7" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="8" t="n"/>
-      <c r="B25" s="7" t="n"/>
-      <c r="C25" s="7" t="n"/>
-      <c r="D25" s="9" t="n"/>
-      <c r="E25" s="7" t="n"/>
-      <c r="F25" s="7" t="n"/>
-      <c r="G25" s="7" t="n"/>
-      <c r="H25" s="7" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="8" t="n"/>
-      <c r="B26" s="7" t="n"/>
-      <c r="C26" s="7" t="n"/>
-      <c r="D26" s="9" t="n"/>
-      <c r="E26" s="7" t="n"/>
-      <c r="F26" s="7" t="n"/>
-      <c r="G26" s="7" t="n"/>
-      <c r="H26" s="7" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="8" t="n"/>
-      <c r="B27" s="7" t="n"/>
-      <c r="C27" s="7" t="n"/>
-      <c r="D27" s="9" t="n"/>
-      <c r="E27" s="7" t="n"/>
-      <c r="F27" s="7" t="n"/>
-      <c r="G27" s="7" t="n"/>
-      <c r="H27" s="7" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="8" t="n"/>
-      <c r="B28" s="7" t="n"/>
-      <c r="C28" s="7" t="n"/>
-      <c r="D28" s="9" t="n"/>
-      <c r="E28" s="7" t="n"/>
-      <c r="F28" s="7" t="n"/>
-      <c r="G28" s="7" t="n"/>
-      <c r="H28" s="7" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="8" t="n"/>
-      <c r="B29" s="7" t="n"/>
-      <c r="C29" s="7" t="n"/>
-      <c r="D29" s="9" t="n"/>
-      <c r="E29" s="7" t="n"/>
-      <c r="F29" s="7" t="n"/>
-      <c r="G29" s="7" t="n"/>
-      <c r="H29" s="7" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="8" t="n"/>
-      <c r="B30" s="7" t="n"/>
-      <c r="C30" s="7" t="n"/>
-      <c r="D30" s="9" t="n"/>
-      <c r="E30" s="7" t="n"/>
-      <c r="F30" s="7" t="n"/>
-      <c r="G30" s="7" t="n"/>
-      <c r="H30" s="7" t="n"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="8" t="n"/>
-      <c r="B31" s="7" t="n"/>
-      <c r="C31" s="7" t="n"/>
-      <c r="D31" s="9" t="n"/>
-      <c r="E31" s="7" t="n"/>
-      <c r="F31" s="7" t="n"/>
-      <c r="G31" s="7" t="n"/>
-      <c r="H31" s="7" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="8" t="n"/>
-      <c r="B32" s="7" t="n"/>
-      <c r="C32" s="7" t="n"/>
-      <c r="D32" s="9" t="n"/>
-      <c r="E32" s="7" t="n"/>
-      <c r="F32" s="7" t="n"/>
-      <c r="G32" s="7" t="n"/>
-      <c r="H32" s="7" t="n"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="8" t="n"/>
-      <c r="B33" s="7" t="n"/>
-      <c r="C33" s="7" t="n"/>
-      <c r="D33" s="9" t="n"/>
-      <c r="E33" s="7" t="n"/>
-      <c r="F33" s="7" t="n"/>
-      <c r="G33" s="7" t="n"/>
-      <c r="H33" s="7" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="8" t="n"/>
-      <c r="B34" s="7" t="n"/>
-      <c r="C34" s="7" t="n"/>
-      <c r="D34" s="9" t="n"/>
-      <c r="E34" s="7" t="n"/>
-      <c r="F34" s="7" t="n"/>
-      <c r="G34" s="7" t="n"/>
-      <c r="H34" s="7" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="8" t="n"/>
-      <c r="B35" s="7" t="n"/>
-      <c r="C35" s="7" t="n"/>
-      <c r="D35" s="9" t="n"/>
-      <c r="E35" s="7" t="n"/>
-      <c r="F35" s="7" t="n"/>
-      <c r="G35" s="7" t="n"/>
-      <c r="H35" s="7" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="8" t="n"/>
-      <c r="B36" s="7" t="n"/>
-      <c r="C36" s="7" t="n"/>
-      <c r="D36" s="9" t="n"/>
-      <c r="E36" s="7" t="n"/>
-      <c r="F36" s="7" t="n"/>
-      <c r="G36" s="7" t="n"/>
-      <c r="H36" s="7" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="8" t="n"/>
-      <c r="B37" s="7" t="n"/>
-      <c r="C37" s="7" t="n"/>
-      <c r="D37" s="9" t="n"/>
-      <c r="E37" s="7" t="n"/>
-      <c r="F37" s="7" t="n"/>
-      <c r="G37" s="7" t="n"/>
-      <c r="H37" s="7" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="8" t="n"/>
-      <c r="B38" s="7" t="n"/>
-      <c r="C38" s="7" t="n"/>
-      <c r="D38" s="9" t="n"/>
-      <c r="E38" s="7" t="n"/>
-      <c r="F38" s="7" t="n"/>
-      <c r="G38" s="7" t="n"/>
-      <c r="H38" s="7" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="8" t="n"/>
-      <c r="B39" s="7" t="n"/>
-      <c r="C39" s="7" t="n"/>
-      <c r="D39" s="9" t="n"/>
-      <c r="E39" s="7" t="n"/>
-      <c r="F39" s="7" t="n"/>
-      <c r="G39" s="7" t="n"/>
-      <c r="H39" s="7" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="8" t="n"/>
-      <c r="B40" s="7" t="n"/>
-      <c r="C40" s="7" t="n"/>
-      <c r="D40" s="9" t="n"/>
-      <c r="E40" s="7" t="n"/>
-      <c r="F40" s="7" t="n"/>
-      <c r="G40" s="7" t="n"/>
-      <c r="H40" s="7" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="8" t="n"/>
-      <c r="B41" s="7" t="n"/>
-      <c r="C41" s="7" t="n"/>
-      <c r="D41" s="9" t="n"/>
-      <c r="E41" s="7" t="n"/>
-      <c r="F41" s="7" t="n"/>
-      <c r="G41" s="7" t="n"/>
-      <c r="H41" s="7" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="8" t="n"/>
-      <c r="B42" s="7" t="n"/>
-      <c r="C42" s="7" t="n"/>
-      <c r="D42" s="9" t="n"/>
-      <c r="E42" s="7" t="n"/>
-      <c r="F42" s="7" t="n"/>
-      <c r="G42" s="7" t="n"/>
-      <c r="H42" s="7" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="8" t="n"/>
-      <c r="B43" s="7" t="n"/>
-      <c r="C43" s="7" t="n"/>
-      <c r="D43" s="9" t="n"/>
-      <c r="E43" s="7" t="n"/>
-      <c r="F43" s="7" t="n"/>
-      <c r="G43" s="7" t="n"/>
-      <c r="H43" s="7" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="8" t="n"/>
-      <c r="B44" s="7" t="n"/>
-      <c r="C44" s="7" t="n"/>
-      <c r="D44" s="9" t="n"/>
-      <c r="E44" s="7" t="n"/>
-      <c r="F44" s="7" t="n"/>
-      <c r="G44" s="7" t="n"/>
-      <c r="H44" s="7" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="8" t="n"/>
-      <c r="B45" s="7" t="n"/>
-      <c r="C45" s="7" t="n"/>
-      <c r="D45" s="9" t="n"/>
-      <c r="E45" s="7" t="n"/>
-      <c r="F45" s="7" t="n"/>
-      <c r="G45" s="7" t="n"/>
-      <c r="H45" s="7" t="n"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="8" t="n"/>
-      <c r="B46" s="7" t="n"/>
-      <c r="C46" s="7" t="n"/>
-      <c r="D46" s="9" t="n"/>
-      <c r="E46" s="7" t="n"/>
-      <c r="F46" s="7" t="n"/>
-      <c r="G46" s="7" t="n"/>
-      <c r="H46" s="7" t="n"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="8" t="n"/>
-      <c r="B47" s="7" t="n"/>
-      <c r="C47" s="7" t="n"/>
-      <c r="D47" s="9" t="n"/>
-      <c r="E47" s="7" t="n"/>
-      <c r="F47" s="7" t="n"/>
-      <c r="G47" s="7" t="n"/>
-      <c r="H47" s="7" t="n"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="8" t="n"/>
-      <c r="B48" s="7" t="n"/>
-      <c r="C48" s="7" t="n"/>
-      <c r="D48" s="9" t="n"/>
-      <c r="E48" s="7" t="n"/>
-      <c r="F48" s="7" t="n"/>
-      <c r="G48" s="7" t="n"/>
-      <c r="H48" s="7" t="n"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="8" t="n"/>
-      <c r="B49" s="7" t="n"/>
-      <c r="C49" s="7" t="n"/>
-      <c r="D49" s="9" t="n"/>
-      <c r="E49" s="7" t="n"/>
-      <c r="F49" s="7" t="n"/>
-      <c r="G49" s="7" t="n"/>
-      <c r="H49" s="7" t="n"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="8" t="n"/>
-      <c r="B50" s="7" t="n"/>
-      <c r="C50" s="7" t="n"/>
-      <c r="D50" s="9" t="n"/>
-      <c r="E50" s="7" t="n"/>
-      <c r="F50" s="7" t="n"/>
-      <c r="G50" s="7" t="n"/>
-      <c r="H50" s="7" t="n"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="8" t="n"/>
-      <c r="B51" s="7" t="n"/>
-      <c r="C51" s="7" t="n"/>
-      <c r="D51" s="9" t="n"/>
-      <c r="E51" s="7" t="n"/>
-      <c r="F51" s="7" t="n"/>
-      <c r="G51" s="7" t="n"/>
-      <c r="H51" s="7" t="n"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="8" t="n"/>
-      <c r="B52" s="7" t="n"/>
-      <c r="C52" s="7" t="n"/>
-      <c r="D52" s="9" t="n"/>
-      <c r="E52" s="7" t="n"/>
-      <c r="F52" s="7" t="n"/>
-      <c r="G52" s="7" t="n"/>
-      <c r="H52" s="7" t="n"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="8" t="n"/>
-      <c r="B53" s="7" t="n"/>
-      <c r="C53" s="7" t="n"/>
-      <c r="D53" s="9" t="n"/>
-      <c r="E53" s="7" t="n"/>
-      <c r="F53" s="7" t="n"/>
-      <c r="G53" s="7" t="n"/>
-      <c r="H53" s="7" t="n"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="8" t="n"/>
-      <c r="B54" s="7" t="n"/>
-      <c r="C54" s="7" t="n"/>
-      <c r="D54" s="9" t="n"/>
-      <c r="E54" s="7" t="n"/>
-      <c r="F54" s="7" t="n"/>
-      <c r="G54" s="7" t="n"/>
-      <c r="H54" s="7" t="n"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="8" t="n"/>
-      <c r="B55" s="7" t="n"/>
-      <c r="C55" s="7" t="n"/>
-      <c r="D55" s="9" t="n"/>
-      <c r="E55" s="7" t="n"/>
-      <c r="F55" s="7" t="n"/>
-      <c r="G55" s="7" t="n"/>
-      <c r="H55" s="7" t="n"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="8" t="n"/>
-      <c r="B56" s="7" t="n"/>
-      <c r="C56" s="7" t="n"/>
-      <c r="D56" s="9" t="n"/>
-      <c r="E56" s="7" t="n"/>
-      <c r="F56" s="7" t="n"/>
-      <c r="G56" s="7" t="n"/>
-      <c r="H56" s="7" t="n"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="8" t="n"/>
-      <c r="B57" s="7" t="n"/>
-      <c r="C57" s="7" t="n"/>
-      <c r="D57" s="9" t="n"/>
-      <c r="E57" s="7" t="n"/>
-      <c r="F57" s="7" t="n"/>
-      <c r="G57" s="7" t="n"/>
-      <c r="H57" s="7" t="n"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="8" t="n"/>
-      <c r="B58" s="7" t="n"/>
-      <c r="C58" s="7" t="n"/>
-      <c r="D58" s="9" t="n"/>
-      <c r="E58" s="7" t="n"/>
-      <c r="F58" s="7" t="n"/>
-      <c r="G58" s="7" t="n"/>
-      <c r="H58" s="7" t="n"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="8" t="n"/>
-      <c r="B59" s="7" t="n"/>
-      <c r="C59" s="7" t="n"/>
-      <c r="D59" s="9" t="n"/>
-      <c r="E59" s="7" t="n"/>
-      <c r="F59" s="7" t="n"/>
-      <c r="G59" s="7" t="n"/>
-      <c r="H59" s="7" t="n"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="8" t="n"/>
-      <c r="B60" s="7" t="n"/>
-      <c r="C60" s="7" t="n"/>
-      <c r="D60" s="9" t="n"/>
-      <c r="E60" s="7" t="n"/>
-      <c r="F60" s="7" t="n"/>
-      <c r="G60" s="7" t="n"/>
-      <c r="H60" s="7" t="n"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="8" t="n"/>
-      <c r="B61" s="7" t="n"/>
-      <c r="C61" s="7" t="n"/>
-      <c r="D61" s="9" t="n"/>
-      <c r="E61" s="7" t="n"/>
-      <c r="F61" s="7" t="n"/>
-      <c r="G61" s="7" t="n"/>
-      <c r="H61" s="7" t="n"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="8" t="n"/>
-      <c r="B62" s="7" t="n"/>
-      <c r="C62" s="7" t="n"/>
-      <c r="D62" s="9" t="n"/>
-      <c r="E62" s="7" t="n"/>
-      <c r="F62" s="7" t="n"/>
-      <c r="G62" s="7" t="n"/>
-      <c r="H62" s="7" t="n"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="8" t="n"/>
-      <c r="B63" s="7" t="n"/>
-      <c r="C63" s="7" t="n"/>
-      <c r="D63" s="9" t="n"/>
-      <c r="E63" s="7" t="n"/>
-      <c r="F63" s="7" t="n"/>
-      <c r="G63" s="7" t="n"/>
-      <c r="H63" s="7" t="n"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="8" t="n"/>
-      <c r="B64" s="7" t="n"/>
-      <c r="C64" s="7" t="n"/>
-      <c r="D64" s="9" t="n"/>
-      <c r="E64" s="7" t="n"/>
-      <c r="F64" s="7" t="n"/>
-      <c r="G64" s="7" t="n"/>
-      <c r="H64" s="7" t="n"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="8" t="n"/>
-      <c r="B65" s="7" t="n"/>
-      <c r="C65" s="7" t="n"/>
-      <c r="D65" s="9" t="n"/>
-      <c r="E65" s="7" t="n"/>
-      <c r="F65" s="7" t="n"/>
-      <c r="G65" s="7" t="n"/>
-      <c r="H65" s="7" t="n"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="8" t="n"/>
-      <c r="B66" s="7" t="n"/>
-      <c r="C66" s="7" t="n"/>
-      <c r="D66" s="9" t="n"/>
-      <c r="E66" s="7" t="n"/>
-      <c r="F66" s="7" t="n"/>
-      <c r="G66" s="7" t="n"/>
-      <c r="H66" s="7" t="n"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="8" t="n"/>
-      <c r="B67" s="7" t="n"/>
-      <c r="C67" s="7" t="n"/>
-      <c r="D67" s="9" t="n"/>
-      <c r="E67" s="7" t="n"/>
-      <c r="F67" s="7" t="n"/>
-      <c r="G67" s="7" t="n"/>
-      <c r="H67" s="7" t="n"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="8" t="n"/>
-      <c r="B68" s="7" t="n"/>
-      <c r="C68" s="7" t="n"/>
-      <c r="D68" s="9" t="n"/>
-      <c r="E68" s="7" t="n"/>
-      <c r="F68" s="7" t="n"/>
-      <c r="G68" s="7" t="n"/>
-      <c r="H68" s="7" t="n"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="8" t="n"/>
-      <c r="B69" s="7" t="n"/>
-      <c r="C69" s="7" t="n"/>
-      <c r="D69" s="9" t="n"/>
-      <c r="E69" s="7" t="n"/>
-      <c r="F69" s="7" t="n"/>
-      <c r="G69" s="7" t="n"/>
-      <c r="H69" s="7" t="n"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="8" t="n"/>
-      <c r="B70" s="7" t="n"/>
-      <c r="C70" s="7" t="n"/>
-      <c r="D70" s="9" t="n"/>
-      <c r="E70" s="7" t="n"/>
-      <c r="F70" s="7" t="n"/>
-      <c r="G70" s="7" t="n"/>
-      <c r="H70" s="7" t="n"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="8" t="n"/>
-      <c r="B71" s="7" t="n"/>
-      <c r="C71" s="7" t="n"/>
-      <c r="D71" s="9" t="n"/>
-      <c r="E71" s="7" t="n"/>
-      <c r="F71" s="7" t="n"/>
-      <c r="G71" s="7" t="n"/>
-      <c r="H71" s="7" t="n"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="8" t="n"/>
-      <c r="B72" s="7" t="n"/>
-      <c r="C72" s="7" t="n"/>
-      <c r="D72" s="9" t="n"/>
-      <c r="E72" s="7" t="n"/>
-      <c r="F72" s="7" t="n"/>
-      <c r="G72" s="7" t="n"/>
-      <c r="H72" s="7" t="n"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="8" t="n"/>
-      <c r="B73" s="7" t="n"/>
-      <c r="C73" s="7" t="n"/>
-      <c r="D73" s="9" t="n"/>
-      <c r="E73" s="7" t="n"/>
-      <c r="F73" s="7" t="n"/>
-      <c r="G73" s="7" t="n"/>
-      <c r="H73" s="7" t="n"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="8" t="n"/>
-      <c r="B74" s="7" t="n"/>
-      <c r="C74" s="7" t="n"/>
-      <c r="D74" s="9" t="n"/>
-      <c r="E74" s="7" t="n"/>
-      <c r="F74" s="7" t="n"/>
-      <c r="G74" s="7" t="n"/>
-      <c r="H74" s="7" t="n"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="8" t="n"/>
-      <c r="B75" s="7" t="n"/>
-      <c r="C75" s="7" t="n"/>
-      <c r="D75" s="9" t="n"/>
-      <c r="E75" s="7" t="n"/>
-      <c r="F75" s="7" t="n"/>
-      <c r="G75" s="7" t="n"/>
-      <c r="H75" s="7" t="n"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="8" t="n"/>
-      <c r="B76" s="7" t="n"/>
-      <c r="C76" s="7" t="n"/>
-      <c r="D76" s="9" t="n"/>
-      <c r="E76" s="7" t="n"/>
-      <c r="F76" s="7" t="n"/>
-      <c r="G76" s="7" t="n"/>
-      <c r="H76" s="7" t="n"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="8" t="n"/>
-      <c r="B77" s="7" t="n"/>
-      <c r="C77" s="7" t="n"/>
-      <c r="D77" s="9" t="n"/>
-      <c r="E77" s="7" t="n"/>
-      <c r="F77" s="7" t="n"/>
-      <c r="G77" s="7" t="n"/>
-      <c r="H77" s="7" t="n"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="8" t="n"/>
-      <c r="B78" s="7" t="n"/>
-      <c r="C78" s="7" t="n"/>
-      <c r="D78" s="9" t="n"/>
-      <c r="E78" s="7" t="n"/>
-      <c r="F78" s="7" t="n"/>
-      <c r="G78" s="7" t="n"/>
-      <c r="H78" s="7" t="n"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="8" t="n"/>
-      <c r="B79" s="7" t="n"/>
-      <c r="C79" s="7" t="n"/>
-      <c r="D79" s="9" t="n"/>
-      <c r="E79" s="7" t="n"/>
-      <c r="F79" s="7" t="n"/>
-      <c r="G79" s="7" t="n"/>
-      <c r="H79" s="7" t="n"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="8" t="n"/>
-      <c r="B80" s="7" t="n"/>
-      <c r="C80" s="7" t="n"/>
-      <c r="D80" s="9" t="n"/>
-      <c r="E80" s="7" t="n"/>
-      <c r="F80" s="7" t="n"/>
-      <c r="G80" s="7" t="n"/>
-      <c r="H80" s="7" t="n"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="8" t="n"/>
-      <c r="B81" s="7" t="n"/>
-      <c r="C81" s="7" t="n"/>
-      <c r="D81" s="9" t="n"/>
-      <c r="E81" s="7" t="n"/>
-      <c r="F81" s="7" t="n"/>
-      <c r="G81" s="7" t="n"/>
-      <c r="H81" s="7" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="8" t="n"/>
-      <c r="B82" s="7" t="n"/>
-      <c r="C82" s="7" t="n"/>
-      <c r="D82" s="9" t="n"/>
-      <c r="E82" s="7" t="n"/>
-      <c r="F82" s="7" t="n"/>
-      <c r="G82" s="7" t="n"/>
-      <c r="H82" s="7" t="n"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="8" t="n"/>
-      <c r="B83" s="7" t="n"/>
-      <c r="C83" s="7" t="n"/>
-      <c r="D83" s="9" t="n"/>
-      <c r="E83" s="7" t="n"/>
-      <c r="F83" s="7" t="n"/>
-      <c r="G83" s="7" t="n"/>
-      <c r="H83" s="7" t="n"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="8" t="n"/>
-      <c r="B84" s="7" t="n"/>
-      <c r="C84" s="7" t="n"/>
-      <c r="D84" s="9" t="n"/>
-      <c r="E84" s="7" t="n"/>
-      <c r="F84" s="7" t="n"/>
-      <c r="G84" s="7" t="n"/>
-      <c r="H84" s="7" t="n"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="8" t="n"/>
-      <c r="B85" s="7" t="n"/>
-      <c r="C85" s="7" t="n"/>
-      <c r="D85" s="9" t="n"/>
-      <c r="E85" s="7" t="n"/>
-      <c r="F85" s="7" t="n"/>
-      <c r="G85" s="7" t="n"/>
-      <c r="H85" s="7" t="n"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="8" t="n"/>
-      <c r="B86" s="7" t="n"/>
-      <c r="C86" s="7" t="n"/>
-      <c r="D86" s="9" t="n"/>
-      <c r="E86" s="7" t="n"/>
-      <c r="F86" s="7" t="n"/>
-      <c r="G86" s="7" t="n"/>
-      <c r="H86" s="7" t="n"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="8" t="n"/>
-      <c r="B87" s="7" t="n"/>
-      <c r="C87" s="7" t="n"/>
-      <c r="D87" s="9" t="n"/>
-      <c r="E87" s="7" t="n"/>
-      <c r="F87" s="7" t="n"/>
-      <c r="G87" s="7" t="n"/>
-      <c r="H87" s="7" t="n"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="8" t="n"/>
-      <c r="B88" s="7" t="n"/>
-      <c r="C88" s="7" t="n"/>
-      <c r="D88" s="9" t="n"/>
-      <c r="E88" s="7" t="n"/>
-      <c r="F88" s="7" t="n"/>
-      <c r="G88" s="7" t="n"/>
-      <c r="H88" s="7" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="8" t="n"/>
-      <c r="B89" s="7" t="n"/>
-      <c r="C89" s="7" t="n"/>
-      <c r="D89" s="9" t="n"/>
-      <c r="E89" s="7" t="n"/>
-      <c r="F89" s="7" t="n"/>
-      <c r="G89" s="7" t="n"/>
-      <c r="H89" s="7" t="n"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="8" t="n"/>
-      <c r="B90" s="7" t="n"/>
-      <c r="C90" s="7" t="n"/>
-      <c r="D90" s="9" t="n"/>
-      <c r="E90" s="7" t="n"/>
-      <c r="F90" s="7" t="n"/>
-      <c r="G90" s="7" t="n"/>
-      <c r="H90" s="7" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="8" t="n"/>
-      <c r="B91" s="7" t="n"/>
-      <c r="C91" s="7" t="n"/>
-      <c r="D91" s="9" t="n"/>
-      <c r="E91" s="7" t="n"/>
-      <c r="F91" s="7" t="n"/>
-      <c r="G91" s="7" t="n"/>
-      <c r="H91" s="7" t="n"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="8" t="n"/>
-      <c r="B92" s="7" t="n"/>
-      <c r="C92" s="7" t="n"/>
-      <c r="D92" s="9" t="n"/>
-      <c r="E92" s="7" t="n"/>
-      <c r="F92" s="7" t="n"/>
-      <c r="G92" s="7" t="n"/>
-      <c r="H92" s="7" t="n"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="8" t="n"/>
-      <c r="B93" s="7" t="n"/>
-      <c r="C93" s="7" t="n"/>
-      <c r="D93" s="9" t="n"/>
-      <c r="E93" s="7" t="n"/>
-      <c r="F93" s="7" t="n"/>
-      <c r="G93" s="7" t="n"/>
-      <c r="H93" s="7" t="n"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="8" t="n"/>
-      <c r="B94" s="7" t="n"/>
-      <c r="C94" s="7" t="n"/>
-      <c r="D94" s="9" t="n"/>
-      <c r="E94" s="7" t="n"/>
-      <c r="F94" s="7" t="n"/>
-      <c r="G94" s="7" t="n"/>
-      <c r="H94" s="7" t="n"/>
-    </row>
-    <row r="95">
-      <c r="A95" s="8" t="n"/>
-      <c r="B95" s="7" t="n"/>
-      <c r="C95" s="7" t="n"/>
-      <c r="D95" s="9" t="n"/>
-      <c r="E95" s="7" t="n"/>
-      <c r="F95" s="7" t="n"/>
-      <c r="G95" s="7" t="n"/>
-      <c r="H95" s="7" t="n"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="8" t="n"/>
-      <c r="B96" s="7" t="n"/>
-      <c r="C96" s="7" t="n"/>
-      <c r="D96" s="9" t="n"/>
-      <c r="E96" s="7" t="n"/>
-      <c r="F96" s="7" t="n"/>
-      <c r="G96" s="7" t="n"/>
-      <c r="H96" s="7" t="n"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="8" t="n"/>
-      <c r="B97" s="7" t="n"/>
-      <c r="C97" s="7" t="n"/>
-      <c r="D97" s="9" t="n"/>
-      <c r="E97" s="7" t="n"/>
-      <c r="F97" s="7" t="n"/>
-      <c r="G97" s="7" t="n"/>
-      <c r="H97" s="7" t="n"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="8" t="n"/>
-      <c r="B98" s="7" t="n"/>
-      <c r="C98" s="7" t="n"/>
-      <c r="D98" s="9" t="n"/>
-      <c r="E98" s="7" t="n"/>
-      <c r="F98" s="7" t="n"/>
-      <c r="G98" s="7" t="n"/>
-      <c r="H98" s="7" t="n"/>
-    </row>
-    <row r="99">
-      <c r="A99" s="8" t="n"/>
-      <c r="B99" s="7" t="n"/>
-      <c r="C99" s="7" t="n"/>
-      <c r="D99" s="9" t="n"/>
-      <c r="E99" s="7" t="n"/>
-      <c r="F99" s="7" t="n"/>
-      <c r="G99" s="7" t="n"/>
-      <c r="H99" s="7" t="n"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="8" t="n"/>
-      <c r="B100" s="7" t="n"/>
-      <c r="C100" s="7" t="n"/>
-      <c r="D100" s="9" t="n"/>
-      <c r="E100" s="7" t="n"/>
-      <c r="F100" s="7" t="n"/>
-      <c r="G100" s="7" t="n"/>
-      <c r="H100" s="7" t="n"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="8" t="n"/>
-      <c r="B101" s="7" t="n"/>
-      <c r="C101" s="7" t="n"/>
-      <c r="D101" s="9" t="n"/>
-      <c r="E101" s="7" t="n"/>
-      <c r="F101" s="7" t="n"/>
-      <c r="G101" s="7" t="n"/>
-      <c r="H101" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5876,10 +4976,11 @@
     <col width="14" customWidth="1" min="10" max="10"/>
     <col width="14" customWidth="1" min="11" max="11"/>
     <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>CONTO ECONOMICO INDUSTRIALE PER UNITÀ OPERATIVA</t>
         </is>
@@ -5943,366 +5044,376 @@
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
+          <t>KCP</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
           <t>TOTALE</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="inlineStr"/>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr"/>
+      <c r="B4" s="9" t="inlineStr">
         <is>
           <t>RICAVI</t>
         </is>
       </c>
-      <c r="C4" s="11" t="n"/>
-      <c r="D4" s="11" t="n"/>
-      <c r="E4" s="11" t="n"/>
-      <c r="F4" s="11" t="n"/>
-      <c r="G4" s="11" t="n"/>
-      <c r="H4" s="11" t="n"/>
-      <c r="I4" s="11" t="n"/>
-      <c r="J4" s="11" t="n"/>
-      <c r="K4" s="11" t="n"/>
-      <c r="L4" s="11" t="n"/>
+      <c r="C4" s="9" t="n"/>
+      <c r="D4" s="9" t="n"/>
+      <c r="E4" s="9" t="n"/>
+      <c r="F4" s="9" t="n"/>
+      <c r="G4" s="9" t="n"/>
+      <c r="H4" s="9" t="n"/>
+      <c r="I4" s="9" t="n"/>
+      <c r="J4" s="9" t="n"/>
+      <c r="K4" s="9" t="n"/>
+      <c r="L4" s="9" t="n"/>
+      <c r="M4" s="9" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>R01</t>
         </is>
       </c>
-      <c r="B5" s="12" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>Ricavi da convenzione SSN/ASP - Degenza</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>R02</t>
         </is>
       </c>
-      <c r="B6" s="12" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>Ricavi da convenzione SSN/ASP - Ambulatoriale</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>R03</t>
         </is>
       </c>
-      <c r="B7" s="12" t="inlineStr">
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>Ricavi da convenzione SSN/ASP - Laboratorio</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>R04</t>
         </is>
       </c>
-      <c r="B8" s="12" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>Ricavi privati/solvenza - Degenza</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="inlineStr">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>R05</t>
         </is>
       </c>
-      <c r="B9" s="12" t="inlineStr">
+      <c r="B9" s="10" t="inlineStr">
         <is>
           <t>Ricavi privati/solvenza - Pacchetti comfort</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>R06</t>
         </is>
       </c>
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t>Ricavi privati/solvenza - Ambulatoriale/Laboratorio</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="inlineStr">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>R07</t>
         </is>
       </c>
-      <c r="B11" s="12" t="inlineStr">
+      <c r="B11" s="10" t="inlineStr">
         <is>
           <t>Altri ricavi (affitti, rimborsi, contributi)</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="n"/>
-      <c r="B12" s="14" t="inlineStr">
+      <c r="A12" s="11" t="n"/>
+      <c r="B12" s="12" t="inlineStr">
         <is>
           <t>TOTALE RICAVI</t>
         </is>
       </c>
-      <c r="C12" s="13" t="n"/>
-      <c r="D12" s="13" t="n"/>
-      <c r="E12" s="13" t="n"/>
-      <c r="F12" s="13" t="n"/>
-      <c r="G12" s="13" t="n"/>
-      <c r="H12" s="13" t="n"/>
-      <c r="I12" s="13" t="n"/>
-      <c r="J12" s="13" t="n"/>
-      <c r="K12" s="13" t="n"/>
-      <c r="L12" s="13" t="n"/>
+      <c r="C12" s="11" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="11" t="n"/>
+      <c r="F12" s="11" t="n"/>
+      <c r="G12" s="11" t="n"/>
+      <c r="H12" s="11" t="n"/>
+      <c r="I12" s="11" t="n"/>
+      <c r="J12" s="11" t="n"/>
+      <c r="K12" s="11" t="n"/>
+      <c r="L12" s="11" t="n"/>
+      <c r="M12" s="11" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="n"/>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="9" t="inlineStr">
         <is>
           <t>COSTI DIRETTI</t>
         </is>
       </c>
-      <c r="C14" s="11" t="n"/>
-      <c r="D14" s="11" t="n"/>
-      <c r="E14" s="11" t="n"/>
-      <c r="F14" s="11" t="n"/>
-      <c r="G14" s="11" t="n"/>
-      <c r="H14" s="11" t="n"/>
-      <c r="I14" s="11" t="n"/>
-      <c r="J14" s="11" t="n"/>
-      <c r="K14" s="11" t="n"/>
-      <c r="L14" s="11" t="n"/>
+      <c r="C14" s="9" t="n"/>
+      <c r="D14" s="9" t="n"/>
+      <c r="E14" s="9" t="n"/>
+      <c r="F14" s="9" t="n"/>
+      <c r="G14" s="9" t="n"/>
+      <c r="H14" s="9" t="n"/>
+      <c r="I14" s="9" t="n"/>
+      <c r="J14" s="9" t="n"/>
+      <c r="K14" s="9" t="n"/>
+      <c r="L14" s="9" t="n"/>
+      <c r="M14" s="9" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="inlineStr">
+      <c r="A15" s="10" t="inlineStr">
         <is>
           <t>CD01</t>
         </is>
       </c>
-      <c r="B15" s="12" t="inlineStr">
+      <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Personale - Medici</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="inlineStr">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>CD02</t>
         </is>
       </c>
-      <c r="B16" s="12" t="inlineStr">
+      <c r="B16" s="10" t="inlineStr">
         <is>
           <t>Personale - Infermieri</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>CD03</t>
         </is>
       </c>
-      <c r="B17" s="12" t="inlineStr">
+      <c r="B17" s="10" t="inlineStr">
         <is>
           <t>Personale - OSS/Ausiliari</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="inlineStr">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>CD04</t>
         </is>
       </c>
-      <c r="B18" s="12" t="inlineStr">
+      <c r="B18" s="10" t="inlineStr">
         <is>
           <t>Personale - Tecnici (lab, rad, FKT)</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="inlineStr">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>CD05</t>
         </is>
       </c>
-      <c r="B19" s="12" t="inlineStr">
+      <c r="B19" s="10" t="inlineStr">
         <is>
           <t>Personale - Amministrativi di struttura</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="inlineStr">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>CD10</t>
         </is>
       </c>
-      <c r="B20" s="12" t="inlineStr">
+      <c r="B20" s="10" t="inlineStr">
         <is>
           <t>Farmaci e presidi sanitari</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="inlineStr">
+      <c r="A21" s="10" t="inlineStr">
         <is>
           <t>CD11</t>
         </is>
       </c>
-      <c r="B21" s="12" t="inlineStr">
+      <c r="B21" s="10" t="inlineStr">
         <is>
           <t>Materiale diagnostico</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="inlineStr">
+      <c r="A22" s="10" t="inlineStr">
         <is>
           <t>CD12</t>
         </is>
       </c>
-      <c r="B22" s="12" t="inlineStr">
+      <c r="B22" s="10" t="inlineStr">
         <is>
           <t>Vitto (gestione interna)</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="inlineStr">
+      <c r="A23" s="10" t="inlineStr">
         <is>
           <t>CD13</t>
         </is>
       </c>
-      <c r="B23" s="12" t="inlineStr">
+      <c r="B23" s="10" t="inlineStr">
         <is>
           <t>Altri materiali di consumo</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="inlineStr">
+      <c r="A24" s="10" t="inlineStr">
         <is>
           <t>CD20</t>
         </is>
       </c>
-      <c r="B24" s="12" t="inlineStr">
+      <c r="B24" s="10" t="inlineStr">
         <is>
           <t>Lavanderia</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="inlineStr">
+      <c r="A25" s="10" t="inlineStr">
         <is>
           <t>CD21</t>
         </is>
       </c>
-      <c r="B25" s="12" t="inlineStr">
+      <c r="B25" s="10" t="inlineStr">
         <is>
           <t>Pulizie</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12" t="inlineStr">
+      <c r="A26" s="10" t="inlineStr">
         <is>
           <t>CD22</t>
         </is>
       </c>
-      <c r="B26" s="12" t="inlineStr">
+      <c r="B26" s="10" t="inlineStr">
         <is>
           <t>Manutenzioni ordinarie</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="12" t="inlineStr">
+      <c r="A27" s="10" t="inlineStr">
         <is>
           <t>CD23</t>
         </is>
       </c>
-      <c r="B27" s="12" t="inlineStr">
+      <c r="B27" s="10" t="inlineStr">
         <is>
           <t>Utenze (quota struttura)</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="12" t="inlineStr">
+      <c r="A28" s="10" t="inlineStr">
         <is>
           <t>CD24</t>
         </is>
       </c>
-      <c r="B28" s="12" t="inlineStr">
+      <c r="B28" s="10" t="inlineStr">
         <is>
           <t>Consulenze sanitarie esterne</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="inlineStr">
+      <c r="A29" s="10" t="inlineStr">
         <is>
           <t>CD30</t>
         </is>
       </c>
-      <c r="B29" s="12" t="inlineStr">
+      <c r="B29" s="10" t="inlineStr">
         <is>
           <t>Ammortamenti attrezzature e arredi</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13" t="n"/>
-      <c r="B30" s="14" t="inlineStr">
+      <c r="A30" s="11" t="n"/>
+      <c r="B30" s="12" t="inlineStr">
         <is>
           <t>TOTALE COSTI DIRETTI</t>
         </is>
       </c>
-      <c r="C30" s="13" t="n"/>
-      <c r="D30" s="13" t="n"/>
-      <c r="E30" s="13" t="n"/>
-      <c r="F30" s="13" t="n"/>
-      <c r="G30" s="13" t="n"/>
-      <c r="H30" s="13" t="n"/>
-      <c r="I30" s="13" t="n"/>
-      <c r="J30" s="13" t="n"/>
-      <c r="K30" s="13" t="n"/>
-      <c r="L30" s="13" t="n"/>
+      <c r="C30" s="11" t="n"/>
+      <c r="D30" s="11" t="n"/>
+      <c r="E30" s="11" t="n"/>
+      <c r="F30" s="11" t="n"/>
+      <c r="G30" s="11" t="n"/>
+      <c r="H30" s="11" t="n"/>
+      <c r="I30" s="11" t="n"/>
+      <c r="J30" s="11" t="n"/>
+      <c r="K30" s="11" t="n"/>
+      <c r="L30" s="11" t="n"/>
+      <c r="M30" s="11" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="n"/>
-      <c r="B32" s="16" t="inlineStr">
+      <c r="A32" s="13" t="n"/>
+      <c r="B32" s="14" t="inlineStr">
         <is>
           <t>MOL INDUSTRIALE (MOL-I)</t>
         </is>
       </c>
-      <c r="C32" s="15" t="n"/>
-      <c r="D32" s="15" t="n"/>
-      <c r="E32" s="15" t="n"/>
-      <c r="F32" s="15" t="n"/>
-      <c r="G32" s="15" t="n"/>
-      <c r="H32" s="15" t="n"/>
-      <c r="I32" s="15" t="n"/>
-      <c r="J32" s="15" t="n"/>
-      <c r="K32" s="15" t="n"/>
-      <c r="L32" s="15" t="n"/>
+      <c r="C32" s="13" t="n"/>
+      <c r="D32" s="13" t="n"/>
+      <c r="E32" s="13" t="n"/>
+      <c r="F32" s="13" t="n"/>
+      <c r="G32" s="13" t="n"/>
+      <c r="H32" s="13" t="n"/>
+      <c r="I32" s="13" t="n"/>
+      <c r="J32" s="13" t="n"/>
+      <c r="K32" s="13" t="n"/>
+      <c r="L32" s="13" t="n"/>
+      <c r="M32" s="13" t="n"/>
     </row>
     <row r="33">
-      <c r="B33" s="17" t="inlineStr">
+      <c r="B33" s="15" t="inlineStr">
         <is>
           <t>MARGINE % INDUSTRIALE</t>
         </is>
@@ -6342,10 +5453,11 @@
     <col width="14" customWidth="1" min="10" max="10"/>
     <col width="14" customWidth="1" min="11" max="11"/>
     <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>CONTO ECONOMICO GESTIONALE PER UNITÀ OPERATIVA</t>
         </is>
@@ -6409,34 +5521,40 @@
       </c>
       <c r="L3" s="1" t="inlineStr">
         <is>
+          <t>KCP</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
           <t>TOTALE</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="18" t="inlineStr">
+      <c r="B4" s="16" t="inlineStr">
         <is>
           <t>MOL INDUSTRIALE (da CE Industriale)</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="n"/>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="A6" s="9" t="n"/>
+      <c r="B6" s="9" t="inlineStr">
         <is>
           <t>COSTI SEDE ALLOCATI</t>
         </is>
       </c>
-      <c r="C6" s="11" t="n"/>
-      <c r="D6" s="11" t="n"/>
-      <c r="E6" s="11" t="n"/>
-      <c r="F6" s="11" t="n"/>
-      <c r="G6" s="11" t="n"/>
-      <c r="H6" s="11" t="n"/>
-      <c r="I6" s="11" t="n"/>
-      <c r="J6" s="11" t="n"/>
-      <c r="K6" s="11" t="n"/>
-      <c r="L6" s="11" t="n"/>
+      <c r="C6" s="9" t="n"/>
+      <c r="D6" s="9" t="n"/>
+      <c r="E6" s="9" t="n"/>
+      <c r="F6" s="9" t="n"/>
+      <c r="G6" s="9" t="n"/>
+      <c r="H6" s="9" t="n"/>
+      <c r="I6" s="9" t="n"/>
+      <c r="J6" s="9" t="n"/>
+      <c r="K6" s="9" t="n"/>
+      <c r="L6" s="9" t="n"/>
+      <c r="M6" s="9" t="n"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6547,65 +5665,68 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="n"/>
-      <c r="B16" s="20" t="inlineStr">
+      <c r="A16" s="17" t="n"/>
+      <c r="B16" s="18" t="inlineStr">
         <is>
           <t>TOTALE COSTI SEDE ALLOCATI</t>
         </is>
       </c>
-      <c r="C16" s="19" t="n"/>
-      <c r="D16" s="19" t="n"/>
-      <c r="E16" s="19" t="n"/>
-      <c r="F16" s="19" t="n"/>
-      <c r="G16" s="19" t="n"/>
-      <c r="H16" s="19" t="n"/>
-      <c r="I16" s="19" t="n"/>
-      <c r="J16" s="19" t="n"/>
-      <c r="K16" s="19" t="n"/>
-      <c r="L16" s="19" t="n"/>
+      <c r="C16" s="17" t="n"/>
+      <c r="D16" s="17" t="n"/>
+      <c r="E16" s="17" t="n"/>
+      <c r="F16" s="17" t="n"/>
+      <c r="G16" s="17" t="n"/>
+      <c r="H16" s="17" t="n"/>
+      <c r="I16" s="17" t="n"/>
+      <c r="J16" s="17" t="n"/>
+      <c r="K16" s="17" t="n"/>
+      <c r="L16" s="17" t="n"/>
+      <c r="M16" s="17" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="21" t="n"/>
-      <c r="B18" s="22" t="inlineStr">
+      <c r="A18" s="19" t="n"/>
+      <c r="B18" s="20" t="inlineStr">
         <is>
           <t>MOL GESTIONALE (MOL-G)</t>
         </is>
       </c>
-      <c r="C18" s="21" t="n"/>
-      <c r="D18" s="21" t="n"/>
-      <c r="E18" s="21" t="n"/>
-      <c r="F18" s="21" t="n"/>
-      <c r="G18" s="21" t="n"/>
-      <c r="H18" s="21" t="n"/>
-      <c r="I18" s="21" t="n"/>
-      <c r="J18" s="21" t="n"/>
-      <c r="K18" s="21" t="n"/>
-      <c r="L18" s="21" t="n"/>
+      <c r="C18" s="19" t="n"/>
+      <c r="D18" s="19" t="n"/>
+      <c r="E18" s="19" t="n"/>
+      <c r="F18" s="19" t="n"/>
+      <c r="G18" s="19" t="n"/>
+      <c r="H18" s="19" t="n"/>
+      <c r="I18" s="19" t="n"/>
+      <c r="J18" s="19" t="n"/>
+      <c r="K18" s="19" t="n"/>
+      <c r="L18" s="19" t="n"/>
+      <c r="M18" s="19" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="17" t="inlineStr">
+      <c r="B19" s="15" t="inlineStr">
         <is>
           <t>MARGINE % GESTIONALE</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="n"/>
-      <c r="B21" s="11" t="inlineStr">
+      <c r="A21" s="9" t="n"/>
+      <c r="B21" s="9" t="inlineStr">
         <is>
           <t>ALTRI COSTI</t>
         </is>
       </c>
-      <c r="C21" s="11" t="n"/>
-      <c r="D21" s="11" t="n"/>
-      <c r="E21" s="11" t="n"/>
-      <c r="F21" s="11" t="n"/>
-      <c r="G21" s="11" t="n"/>
-      <c r="H21" s="11" t="n"/>
-      <c r="I21" s="11" t="n"/>
-      <c r="J21" s="11" t="n"/>
-      <c r="K21" s="11" t="n"/>
-      <c r="L21" s="11" t="n"/>
+      <c r="C21" s="9" t="n"/>
+      <c r="D21" s="9" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+      <c r="G21" s="9" t="n"/>
+      <c r="H21" s="9" t="n"/>
+      <c r="I21" s="9" t="n"/>
+      <c r="J21" s="9" t="n"/>
+      <c r="K21" s="9" t="n"/>
+      <c r="L21" s="9" t="n"/>
+      <c r="M21" s="9" t="n"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -6644,22 +5765,23 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="n"/>
-      <c r="B26" s="23" t="inlineStr">
+      <c r="A26" s="11" t="n"/>
+      <c r="B26" s="21" t="inlineStr">
         <is>
           <t>RISULTATO NETTO UNITÀ OPERATIVA</t>
         </is>
       </c>
-      <c r="C26" s="13" t="n"/>
-      <c r="D26" s="13" t="n"/>
-      <c r="E26" s="13" t="n"/>
-      <c r="F26" s="13" t="n"/>
-      <c r="G26" s="13" t="n"/>
-      <c r="H26" s="13" t="n"/>
-      <c r="I26" s="13" t="n"/>
-      <c r="J26" s="13" t="n"/>
-      <c r="K26" s="13" t="n"/>
-      <c r="L26" s="13" t="n"/>
+      <c r="C26" s="11" t="n"/>
+      <c r="D26" s="11" t="n"/>
+      <c r="E26" s="11" t="n"/>
+      <c r="F26" s="11" t="n"/>
+      <c r="G26" s="11" t="n"/>
+      <c r="H26" s="11" t="n"/>
+      <c r="I26" s="11" t="n"/>
+      <c r="J26" s="11" t="n"/>
+      <c r="K26" s="11" t="n"/>
+      <c r="L26" s="11" t="n"/>
+      <c r="M26" s="11" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>